<commit_message>
Excel to Map and Maven Cucumbe Reports
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/ExelenterEmployeesList.xlsx
+++ b/src/test/resources/testdata/ExelenterEmployeesList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/TestNGFrameworkB1/src/test/resources/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/CucumberB1/src/test/resources/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CFFB684-5024-DB4C-8171-FA4A523C08B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A3ADD9-1C25-F24B-84F4-32121EBA23BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7640" yWindow="-16300" windowWidth="17800" windowHeight="13980" xr2:uid="{7A12BD58-98C9-E048-8107-5573E8AB6C07}"/>
+    <workbookView xWindow="-14300" yWindow="-19000" windowWidth="24320" windowHeight="16100" xr2:uid="{7A12BD58-98C9-E048-8107-5573E8AB6C07}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Firstname</t>
   </si>
@@ -152,6 +152,18 @@
   </si>
   <si>
     <t>johnSmith1332</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>alexJordan</t>
+  </si>
+  <si>
+    <t>jordan@_2023!!!</t>
   </si>
 </sst>
 </file>
@@ -585,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57988F14-CEFA-C548-B8A8-EA00BB470A14}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,10 +681,25 @@
         <v>15</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D5" r:id="rId1" xr:uid="{413597BE-98BF-C14F-833A-251922B7289F}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{9C85D388-88D2-A849-926D-1F351D2611D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>